<commit_message>
[WIP] power and main sheet needs to be finished
</commit_message>
<xml_diff>
--- a/BASE/esp32-c6_pin_definitions.xlsx
+++ b/BASE/esp32-c6_pin_definitions.xlsx
@@ -127,7 +127,7 @@
     <t xml:space="preserve">IO8</t>
   </si>
   <si>
-    <t xml:space="preserve">GPIO8</t>
+    <t xml:space="preserve">GPIO8, chip boot mode</t>
   </si>
   <si>
     <t xml:space="preserve">CLK</t>
@@ -175,7 +175,7 @@
     <t xml:space="preserve">IO9</t>
   </si>
   <si>
-    <t xml:space="preserve">GPIO9</t>
+    <t xml:space="preserve">GPIO9, chip boot mode</t>
   </si>
   <si>
     <t xml:space="preserve">GPIO_15</t>
@@ -416,44 +416,48 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -712,741 +716,741 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O17" activeCellId="0" sqref="O17"/>
+      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="80.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="0" width="5.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="80.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="1" width="5.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="3" t="s">
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="3" t="str">
+      <c r="H7" s="4" t="str">
         <f aca="false">E2</f>
         <v>GND</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="5"/>
-      <c r="K7" s="3" t="s">
+      <c r="J7" s="6"/>
+      <c r="K7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L7" s="3" t="str">
+      <c r="L7" s="4" t="str">
         <f aca="false">E29</f>
         <v>GND</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="6" t="n">
+      <c r="B8" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="6" t="s">
+      <c r="C8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="3" t="str">
+      <c r="H8" s="4" t="str">
         <f aca="false">E3</f>
         <v>3V3</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="3" t="n">
+      <c r="J8" s="6"/>
+      <c r="K8" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="L8" s="3" t="str">
+      <c r="L8" s="4" t="str">
         <f aca="false">E28</f>
         <v>RX</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="3" t="str">
+      <c r="H9" s="4" t="str">
         <f aca="false">E4</f>
         <v>EN</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="5"/>
-      <c r="K9" s="3" t="n">
+      <c r="J9" s="6"/>
+      <c r="K9" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="L9" s="3" t="str">
+      <c r="L9" s="4" t="str">
         <f aca="false">E27</f>
         <v>TX</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="3" t="str">
+      <c r="H10" s="4" t="str">
         <f aca="false">E5</f>
         <v>GPIO_0</v>
       </c>
-      <c r="I10" s="3" t="n">
+      <c r="I10" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="3" t="n">
+      <c r="J10" s="6"/>
+      <c r="K10" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="L10" s="3" t="str">
+      <c r="L10" s="4" t="str">
         <f aca="false">E26</f>
         <v>GPIO_6</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="6" t="n">
+      <c r="B11" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="C11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="3" t="str">
+      <c r="H11" s="4" t="str">
         <f aca="false">E6</f>
         <v>GPIO_1</v>
       </c>
-      <c r="I11" s="3" t="n">
+      <c r="I11" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="3" t="n">
+      <c r="J11" s="6"/>
+      <c r="K11" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="L11" s="3" t="str">
+      <c r="L11" s="4" t="str">
         <f aca="false">E25</f>
         <v>GPIO_7</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="6" t="n">
+      <c r="B12" s="7" t="n">
         <v>11</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="C12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="3" t="str">
+      <c r="H12" s="4" t="str">
         <f aca="false">E7</f>
         <v>GPIO_2</v>
       </c>
-      <c r="I12" s="3" t="n">
+      <c r="I12" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="J12" s="5"/>
-      <c r="K12" s="3" t="n">
+      <c r="J12" s="6"/>
+      <c r="K12" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="L12" s="3" t="str">
+      <c r="L12" s="4" t="str">
         <f aca="false">E24</f>
         <v>GPIO_8</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="6" t="n">
+      <c r="B13" s="7" t="n">
         <v>12</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="C13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H13" s="3" t="str">
+      <c r="H13" s="4" t="str">
         <f aca="false">E8</f>
         <v>GPIO_3</v>
       </c>
-      <c r="I13" s="3" t="n">
+      <c r="I13" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="J13" s="5"/>
-      <c r="K13" s="3" t="s">
+      <c r="J13" s="6"/>
+      <c r="K13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="L13" s="3" t="str">
+      <c r="L13" s="4" t="str">
         <f aca="false">E23</f>
         <v>NC</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="7" t="n">
+      <c r="B14" s="8" t="n">
         <v>13</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="7" t="s">
+      <c r="C14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H14" s="3" t="str">
+      <c r="H14" s="4" t="str">
         <f aca="false">E9</f>
         <v>GPIO_4</v>
       </c>
-      <c r="I14" s="3" t="n">
+      <c r="I14" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="J14" s="5"/>
-      <c r="K14" s="3" t="n">
+      <c r="J14" s="6"/>
+      <c r="K14" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="L14" s="3" t="str">
+      <c r="L14" s="4" t="str">
         <f aca="false">E22</f>
         <v>GPIO_9</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="7" t="n">
-        <v>14</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="7" t="s">
+      <c r="B15" s="8" t="n">
+        <v>14</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H15" s="3" t="str">
+      <c r="H15" s="4" t="str">
         <f aca="false">E10</f>
         <v>GPIO_5</v>
       </c>
-      <c r="I15" s="3" t="n">
+      <c r="I15" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="J15" s="5"/>
-      <c r="K15" s="3" t="n">
+      <c r="J15" s="6"/>
+      <c r="K15" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="L15" s="3" t="str">
+      <c r="L15" s="4" t="str">
         <f aca="false">E21</f>
         <v>GPIO_10</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="6" t="n">
+      <c r="B16" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="6" t="s">
+      <c r="C16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H16" s="3" t="str">
+      <c r="H16" s="4" t="str">
         <f aca="false">E11</f>
         <v>CLK</v>
       </c>
-      <c r="I16" s="3" t="n">
+      <c r="I16" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="J16" s="5"/>
-      <c r="K16" s="3" t="n">
+      <c r="J16" s="6"/>
+      <c r="K16" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="L16" s="3" t="str">
+      <c r="L16" s="4" t="str">
         <f aca="false">E20</f>
         <v>GPIO_11</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="8" t="n">
+      <c r="B17" s="9" t="n">
         <v>16</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="8" t="s">
+      <c r="C17" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H17" s="3" t="str">
+      <c r="H17" s="4" t="str">
         <f aca="false">E12</f>
         <v>LATCH</v>
       </c>
-      <c r="I17" s="3" t="n">
+      <c r="I17" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="J17" s="5"/>
-      <c r="K17" s="3" t="n">
+      <c r="J17" s="6"/>
+      <c r="K17" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="L17" s="3" t="str">
+      <c r="L17" s="4" t="str">
         <f aca="false">E19</f>
         <v>GPIO_12</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="8" t="n">
+      <c r="B18" s="9" t="n">
         <v>17</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="8" t="s">
+      <c r="C18" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H18" s="3" t="str">
+      <c r="H18" s="4" t="str">
         <f aca="false">E13</f>
         <v>DATA</v>
       </c>
-      <c r="I18" s="3" t="n">
+      <c r="I18" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="J18" s="5"/>
-      <c r="K18" s="3" t="n">
+      <c r="J18" s="6"/>
+      <c r="K18" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="L18" s="3" t="str">
+      <c r="L18" s="4" t="str">
         <f aca="false">E18</f>
         <v>GPIO_13</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="8" t="n">
+      <c r="B19" s="9" t="n">
         <v>18</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="8" t="s">
+      <c r="C19" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H19" s="3" t="str">
+      <c r="H19" s="4" t="str">
         <f aca="false">E14</f>
         <v>USB_D-</v>
       </c>
-      <c r="I19" s="3" t="n">
+      <c r="I19" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="J19" s="5"/>
-      <c r="K19" s="3" t="n">
+      <c r="J19" s="6"/>
+      <c r="K19" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="L19" s="3" t="str">
+      <c r="L19" s="4" t="str">
         <f aca="false">E17</f>
         <v>GPIO_14</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="8" t="n">
+      <c r="B20" s="9" t="n">
         <v>19</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="8" t="s">
+      <c r="C20" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H20" s="3" t="str">
+      <c r="H20" s="4" t="str">
         <f aca="false">E15</f>
         <v>USB_D+</v>
       </c>
-      <c r="I20" s="3" t="n">
-        <v>14</v>
-      </c>
-      <c r="J20" s="5"/>
-      <c r="K20" s="3" t="n">
+      <c r="I20" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="J20" s="6"/>
+      <c r="K20" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="L20" s="3" t="str">
+      <c r="L20" s="4" t="str">
         <f aca="false">E16</f>
         <v>GPIO_15</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="8" t="n">
+      <c r="B21" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="8" t="s">
+      <c r="C21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="8" t="n">
+      <c r="B22" s="9" t="n">
         <v>21</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="8" t="s">
+      <c r="C22" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E23" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="6" t="n">
+      <c r="B24" s="7" t="n">
         <v>23</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="6" t="s">
+      <c r="C24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="E24" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B25" s="9" t="n">
+      <c r="B25" s="10" t="n">
         <v>24</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="9" t="s">
+      <c r="C25" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B26" s="9" t="n">
+      <c r="B26" s="10" t="n">
         <v>25</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="9" t="s">
+      <c r="C26" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B27" s="2" t="n">
+      <c r="B27" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="C27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="E27" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="2" t="n">
+      <c r="B28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="C28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E28" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[FLOORPLAN_DONE] working on routing
</commit_message>
<xml_diff>
--- a/BASE/esp32-c6_pin_definitions.xlsx
+++ b/BASE/esp32-c6_pin_definitions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="87">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -70,60 +70,60 @@
     <t xml:space="preserve">MTMS, GPIO4, LP_GPIO4, LP_UART_RXD, ADC1_CH4, FSPIHD</t>
   </si>
   <si>
+    <t xml:space="preserve">GPIO_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTDI, GPIO5, LP_GPIO5, LP_UART_TXD, ADC1_CH5, FSPIWP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESP32-C6 pinnout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTCK, GPIO6, LP_GPIO6, LP_I2C_SDA, ADC1_CH6, FSPICLK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTDO, GPIO7, LP_GPIO7, LP_I2C_SCL, FSPID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO0, XTAL_32K_P, LP_GPIO0, LP_UART_DTRN, ADC1_CH0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO1, XTAL_32K_N, LP_GPIO1, LP_UART_DSRN, ADC1_CH1</t>
+  </si>
+  <si>
     <t xml:space="preserve">GPIO_0</t>
   </si>
   <si>
-    <t xml:space="preserve">IO5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MTDI, GPIO5, LP_GPIO5, LP_UART_TXD, ADC1_CH5, FSPIWP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESP32-C6 pinnout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MTCK, GPIO6, LP_GPIO6, LP_I2C_SDA, ADC1_CH6, FSPICLK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MTDO, GPIO7, LP_GPIO7, LP_I2C_SCL, FSPID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO0, XTAL_32K_P, LP_GPIO0, LP_UART_DTRN, ADC1_CH0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO1, XTAL_32K_N, LP_GPIO1, LP_UART_DSRN, ADC1_CH1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO_5</t>
-  </si>
-  <si>
     <t xml:space="preserve">IO8</t>
   </si>
   <si>
@@ -160,7 +160,7 @@
     <t xml:space="preserve">GPIO12, USB_D-</t>
   </si>
   <si>
-    <t xml:space="preserve">USB_D-</t>
+    <t xml:space="preserve">USB_N</t>
   </si>
   <si>
     <t xml:space="preserve">IO13</t>
@@ -169,7 +169,7 @@
     <t xml:space="preserve">GPIO13, USB_D+</t>
   </si>
   <si>
-    <t xml:space="preserve">USB_D+</t>
+    <t xml:space="preserve">USB_P</t>
   </si>
   <si>
     <t xml:space="preserve">IO9</t>
@@ -178,84 +178,81 @@
     <t xml:space="preserve">GPIO9, chip boot mode</t>
   </si>
   <si>
+    <t xml:space="preserve">GPIO_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO18, SDIO_CMD, FSPICS2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO19, SDIO_CLK, FSPICS3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO20, SDIO_DATA0, FSPICS4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO21, SDIO_DATA1, FSPICS5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO22, SDIO_DATA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO_12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO23, SDIO_DATA3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO_13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">—</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO_14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RXD0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U0RXD, GPIO17, FSPICS1</t>
+  </si>
+  <si>
     <t xml:space="preserve">GPIO_15</t>
   </si>
   <si>
-    <t xml:space="preserve">IO18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO18, SDIO_CMD, FSPICS2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO_14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO19, SDIO_CLK, FSPICS3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO_13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO20, SDIO_DATA0, FSPICS4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO_12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO21, SDIO_DATA1, FSPICS5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO_11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO22, SDIO_DATA2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO_10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO23, SDIO_DATA3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO_9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">—</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO_8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RXD0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U0RXD, GPIO17, FSPICS1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO_7</t>
-  </si>
-  <si>
     <t xml:space="preserve">TXD0</t>
   </si>
   <si>
@@ -271,16 +268,16 @@
     <t xml:space="preserve">GPIO3, LP_GPIO3, LP_UART_CTSN, ADC1_CH3</t>
   </si>
   <si>
+    <t xml:space="preserve">RX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO2, LP_GPIO2, LP_UART_RTSN, ADC1_CH2, FSPIQ</t>
+  </si>
+  <si>
     <t xml:space="preserve">TX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO2, LP_GPIO2, LP_UART_RTSN, ADC1_CH2, FSPIQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RX</t>
   </si>
   <si>
     <t xml:space="preserve">EPAD</t>
@@ -715,8 +712,8 @@
   </sheetPr>
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -900,7 +897,7 @@
       </c>
       <c r="L8" s="4" t="str">
         <f aca="false">E28</f>
-        <v>RX</v>
+        <v>TX</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -932,7 +929,7 @@
       </c>
       <c r="L9" s="4" t="str">
         <f aca="false">E27</f>
-        <v>TX</v>
+        <v>RX</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -953,7 +950,7 @@
       </c>
       <c r="H10" s="4" t="str">
         <f aca="false">E5</f>
-        <v>GPIO_0</v>
+        <v>GPIO_5</v>
       </c>
       <c r="I10" s="4" t="n">
         <v>4</v>
@@ -985,7 +982,7 @@
       </c>
       <c r="H11" s="4" t="str">
         <f aca="false">E6</f>
-        <v>GPIO_1</v>
+        <v>GPIO_4</v>
       </c>
       <c r="I11" s="4" t="n">
         <v>5</v>
@@ -996,7 +993,7 @@
       </c>
       <c r="L11" s="4" t="str">
         <f aca="false">E25</f>
-        <v>GPIO_7</v>
+        <v>GPIO_15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1017,7 +1014,7 @@
       </c>
       <c r="H12" s="4" t="str">
         <f aca="false">E7</f>
-        <v>GPIO_2</v>
+        <v>GPIO_3</v>
       </c>
       <c r="I12" s="4" t="n">
         <v>6</v>
@@ -1028,7 +1025,7 @@
       </c>
       <c r="L12" s="4" t="str">
         <f aca="false">E24</f>
-        <v>GPIO_8</v>
+        <v>GPIO_14</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1049,7 +1046,7 @@
       </c>
       <c r="H13" s="4" t="str">
         <f aca="false">E8</f>
-        <v>GPIO_3</v>
+        <v>GPIO_2</v>
       </c>
       <c r="I13" s="4" t="n">
         <v>7</v>
@@ -1081,7 +1078,7 @@
       </c>
       <c r="H14" s="4" t="str">
         <f aca="false">E9</f>
-        <v>GPIO_4</v>
+        <v>GPIO_1</v>
       </c>
       <c r="I14" s="4" t="n">
         <v>8</v>
@@ -1092,7 +1089,7 @@
       </c>
       <c r="L14" s="4" t="str">
         <f aca="false">E22</f>
-        <v>GPIO_9</v>
+        <v>GPIO_13</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1113,7 +1110,7 @@
       </c>
       <c r="H15" s="4" t="str">
         <f aca="false">E10</f>
-        <v>GPIO_5</v>
+        <v>GPIO_0</v>
       </c>
       <c r="I15" s="4" t="n">
         <v>9</v>
@@ -1124,7 +1121,7 @@
       </c>
       <c r="L15" s="4" t="str">
         <f aca="false">E21</f>
-        <v>GPIO_10</v>
+        <v>GPIO_12</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1173,7 +1170,7 @@
         <v>54</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H17" s="4" t="str">
         <f aca="false">E12</f>
@@ -1188,12 +1185,12 @@
       </c>
       <c r="L17" s="4" t="str">
         <f aca="false">E19</f>
-        <v>GPIO_12</v>
+        <v>GPIO_10</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="9" t="n">
         <v>17</v>
@@ -1202,10 +1199,10 @@
         <v>14</v>
       </c>
       <c r="D18" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="H18" s="4" t="str">
         <f aca="false">E13</f>
@@ -1220,12 +1217,12 @@
       </c>
       <c r="L18" s="4" t="str">
         <f aca="false">E18</f>
-        <v>GPIO_13</v>
+        <v>GPIO_9</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="9" t="n">
         <v>18</v>
@@ -1234,14 +1231,14 @@
         <v>14</v>
       </c>
       <c r="D19" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="H19" s="4" t="str">
         <f aca="false">E14</f>
-        <v>USB_D-</v>
+        <v>USB_N</v>
       </c>
       <c r="I19" s="4" t="n">
         <v>13</v>
@@ -1252,12 +1249,12 @@
       </c>
       <c r="L19" s="4" t="str">
         <f aca="false">E17</f>
-        <v>GPIO_14</v>
+        <v>GPIO_8</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="9" t="n">
         <v>19</v>
@@ -1266,14 +1263,14 @@
         <v>14</v>
       </c>
       <c r="D20" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="H20" s="4" t="str">
         <f aca="false">E15</f>
-        <v>USB_D+</v>
+        <v>USB_P</v>
       </c>
       <c r="I20" s="4" t="n">
         <v>14</v>
@@ -1284,12 +1281,12 @@
       </c>
       <c r="L20" s="4" t="str">
         <f aca="false">E16</f>
-        <v>GPIO_15</v>
+        <v>GPIO_8</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B21" s="9" t="n">
         <v>20</v>
@@ -1298,15 +1295,15 @@
         <v>14</v>
       </c>
       <c r="D21" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B22" s="9" t="n">
         <v>21</v>
@@ -1315,10 +1312,10 @@
         <v>14</v>
       </c>
       <c r="D22" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1329,7 +1326,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>43</v>
@@ -1340,7 +1337,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B24" s="7" t="n">
         <v>23</v>
@@ -1349,15 +1346,15 @@
         <v>14</v>
       </c>
       <c r="D24" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B25" s="10" t="n">
         <v>24</v>
@@ -1366,15 +1363,15 @@
         <v>14</v>
       </c>
       <c r="D25" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B26" s="10" t="n">
         <v>25</v>
@@ -1383,15 +1380,15 @@
         <v>14</v>
       </c>
       <c r="D26" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B27" s="3" t="n">
         <v>26</v>
@@ -1400,15 +1397,15 @@
         <v>14</v>
       </c>
       <c r="D27" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B28" s="3" t="n">
         <v>27</v>
@@ -1417,10 +1414,10 @@
         <v>14</v>
       </c>
       <c r="D28" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1442,7 +1439,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>29</v>

</xml_diff>